<commit_message>
Trying to fix issues with Hess running the code
</commit_message>
<xml_diff>
--- a/Code/Data/LP_Umps2021.xlsx
+++ b/Code/Data/LP_Umps2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/rdardis_student_unimelb_edu_au/Documents/Uni/MSC/2021/Semester2/MAST90050/GroupProject/Mast90050_UmpScheduling/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{793C9527-181C-DE42-B36E-9BB008362F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4BA70E4-6051-4888-A0CC-C07EA54F7E93}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{793C9527-181C-DE42-B36E-9BB008362F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18710648-2D73-455F-A6DF-DBC5DBEFB575}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="438">
   <si>
     <t>Last Name</t>
   </si>
@@ -1182,9 +1182,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>!0:00</t>
   </si>
   <si>
     <t>Langford, Ellis</t>
@@ -2021,10 +2018,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2043,7 @@
         <v>147</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>148</v>
@@ -2066,21 +2063,21 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G2:H2)</f>
+        <f t="shared" ref="A2:A33" si="0">_xlfn.TEXTJOIN(", ",1,G2:H2)</f>
         <v>Brown, Henry</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34" t="s">
         <v>190</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>24</v>
@@ -2091,14 +2088,14 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G3:H3)</f>
+        <f t="shared" si="0"/>
         <v>Collopy, John</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -2114,14 +2111,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G4:H4)</f>
+        <f t="shared" si="0"/>
         <v>Dardis, Richard</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
@@ -2137,14 +2134,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G5:H5)</f>
+        <f t="shared" si="0"/>
         <v>Davis, Adam</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
@@ -2160,19 +2157,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G6:H6)</f>
+        <f t="shared" si="0"/>
         <v>Dodds, Matthew</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>32</v>
@@ -2183,14 +2180,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G7:H7)</f>
+        <f t="shared" si="0"/>
         <v>Dodds, Rosalie</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
@@ -2206,14 +2203,14 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G8:H8)</f>
+        <f t="shared" si="0"/>
         <v>Edwards, Patrick</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -2227,14 +2224,14 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G9:H9)</f>
+        <f t="shared" si="0"/>
         <v>Garrard, Sam</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -2248,14 +2245,14 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G10:H10)</f>
+        <f t="shared" si="0"/>
         <v>Graves, Thomas</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2269,14 +2266,14 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G11:H11)</f>
+        <f t="shared" si="0"/>
         <v>Hain, Matthew</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -2290,14 +2287,14 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G12:H12)</f>
+        <f t="shared" si="0"/>
         <v>Harrison, Lucas</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
@@ -2313,14 +2310,14 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G13:H13)</f>
+        <f t="shared" si="0"/>
         <v>Lefebvre, Benjamin</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2334,14 +2331,14 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G14:H14)</f>
+        <f t="shared" si="0"/>
         <v>Melville, James</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2355,14 +2352,14 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G15:H15)</f>
+        <f t="shared" si="0"/>
         <v>Melville, Lachlan</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2376,14 +2373,14 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G16:H16)</f>
+        <f t="shared" si="0"/>
         <v>Minisini, Enio</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2397,14 +2394,14 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G17:H17)</f>
+        <f t="shared" si="0"/>
         <v>Minisini, Marcus</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2418,20 +2415,20 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G18:H18)</f>
+        <f t="shared" si="0"/>
         <v>Moyle, Ben</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="5"/>
       <c r="G18" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>15</v>
@@ -2439,14 +2436,14 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G19:H19)</f>
+        <f t="shared" si="0"/>
         <v>Nitz, Joshua</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
@@ -2462,14 +2459,14 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G20:H20)</f>
+        <f t="shared" si="0"/>
         <v>Prior, Sam</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
@@ -2485,14 +2482,14 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G21:H21)</f>
+        <f t="shared" si="0"/>
         <v>Purcell, Sebastian</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2506,21 +2503,21 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G22:H22)</f>
+        <f t="shared" si="0"/>
         <v>Scott, Angus</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
         <v>190</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>156</v>
@@ -2531,14 +2528,14 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G23:H23)</f>
+        <f t="shared" si="0"/>
         <v>Stacey, Joshua</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
@@ -2554,14 +2551,14 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G24:H24)</f>
+        <f t="shared" si="0"/>
         <v>Thiele, Benjamin</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C24" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
@@ -2577,14 +2574,14 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G25:H25)</f>
+        <f t="shared" si="0"/>
         <v>Thiele, Jon</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2598,14 +2595,14 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G26:H26)</f>
+        <f t="shared" si="0"/>
         <v>Thornton, Hugo</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C26" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2619,14 +2616,14 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G27:H27)</f>
+        <f t="shared" si="0"/>
         <v>Allen, Luke</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
@@ -2642,14 +2639,14 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G28:H28)</f>
+        <f t="shared" si="0"/>
         <v>Baltutis, Evan</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
@@ -2665,14 +2662,14 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G29:H29)</f>
+        <f t="shared" si="0"/>
         <v>Boulter, Oscar</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
@@ -2688,35 +2685,35 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G30:H30)</f>
+        <f t="shared" si="0"/>
         <v>Cole, Georgi</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
       <c r="G30" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>395</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G31:H31)</f>
+        <f t="shared" si="0"/>
         <v>Cornelius, Ryan</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2730,14 +2727,14 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G32:H32)</f>
+        <f t="shared" si="0"/>
         <v>Ford, Harvey</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
@@ -2753,14 +2750,14 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G33:H33)</f>
+        <f t="shared" si="0"/>
         <v>Hester, Thomas</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
@@ -2776,14 +2773,14 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G34:H34)</f>
+        <f t="shared" ref="A34:A65" si="1">_xlfn.TEXTJOIN(", ",1,G34:H34)</f>
         <v>Hough, Harrison</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2797,14 +2794,14 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G35:H35)</f>
+        <f t="shared" si="1"/>
         <v>Lawton, Cornelius</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
@@ -2820,14 +2817,14 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G36:H36)</f>
+        <f t="shared" si="1"/>
         <v>Minett, Declan</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
@@ -2843,14 +2840,14 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G37:H37)</f>
+        <f t="shared" si="1"/>
         <v>Munro, Nathan</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>185</v>
@@ -2866,14 +2863,14 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G38:H38)</f>
+        <f t="shared" si="1"/>
         <v>Prior, Thomas</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
@@ -2889,14 +2886,14 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G39:H39)</f>
+        <f t="shared" si="1"/>
         <v>Robinson, Ben</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C39" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
@@ -2912,14 +2909,14 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G40:H40)</f>
+        <f t="shared" si="1"/>
         <v>Rogan, Christian</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2933,14 +2930,14 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G41:H41)</f>
+        <f t="shared" si="1"/>
         <v>Sandy, William</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
@@ -2956,35 +2953,35 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G42:H42)</f>
+        <f t="shared" si="1"/>
         <v>Schwarz, Quinn</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G43:H43)</f>
+        <f t="shared" si="1"/>
         <v>Shearer, Edward</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
@@ -3000,14 +2997,14 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G44:H44)</f>
+        <f t="shared" si="1"/>
         <v>Sherry, Matthew</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="19" t="s">
@@ -3023,14 +3020,14 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G45:H45)</f>
+        <f t="shared" si="1"/>
         <v>Sutherland, Tom</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
@@ -3046,14 +3043,14 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G46:H46)</f>
+        <f t="shared" si="1"/>
         <v>Thornton, Conrad</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
@@ -3069,14 +3066,14 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G47:H47)</f>
+        <f t="shared" si="1"/>
         <v>Villiers De Casanove, Gabriel</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
@@ -3092,21 +3089,21 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G48:H48)</f>
+        <f t="shared" si="1"/>
         <v>Walsh, Austin</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
         <v>190</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>140</v>
@@ -3117,14 +3114,14 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G49:H49)</f>
+        <f t="shared" si="1"/>
         <v>Woolley, Michael</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
@@ -3140,21 +3137,21 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G50:H50)</f>
+        <f t="shared" si="1"/>
         <v>Anderson, Callum</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
         <v>190</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>7</v>
@@ -3165,14 +3162,14 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G51:H51)</f>
+        <f t="shared" si="1"/>
         <v>Askew, Freddie</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C51" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>376</v>
@@ -3180,22 +3177,22 @@
       <c r="E51" s="4"/>
       <c r="F51" s="5"/>
       <c r="G51" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="H51" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G52:H52)</f>
+        <f t="shared" si="1"/>
         <v>Bennett, Joel Samuel</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
@@ -3211,14 +3208,14 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G53:H53)</f>
+        <f t="shared" si="1"/>
         <v>Bennett, Nicholas</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
@@ -3234,14 +3231,14 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G54:H54)</f>
+        <f t="shared" si="1"/>
         <v>Bourke, Hayden</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C54" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>376</v>
@@ -3249,22 +3246,22 @@
       <c r="E54" s="4"/>
       <c r="F54" s="5"/>
       <c r="G54" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="H54" s="5" t="s">
         <v>402</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G55:H55)</f>
+        <f t="shared" si="1"/>
         <v>Branagan, Billy</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
@@ -3280,14 +3277,14 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G56:H56)</f>
+        <f t="shared" si="1"/>
         <v>Cox, Owen</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>339</v>
@@ -3303,14 +3300,14 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G57:H57)</f>
+        <f t="shared" si="1"/>
         <v>Davis, Luke</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
@@ -3326,14 +3323,14 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G58:H58)</f>
+        <f t="shared" si="1"/>
         <v>Docherty, Henry Bernard</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>339</v>
@@ -3341,22 +3338,22 @@
       <c r="E58" s="4"/>
       <c r="F58" s="5"/>
       <c r="G58" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="H58" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G59:H59)</f>
+        <f t="shared" si="1"/>
         <v>Florance, Hugh</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -3372,14 +3369,14 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G60:H60)</f>
+        <f t="shared" si="1"/>
         <v>Georgelin, Edward</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -3395,14 +3392,14 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G61:H61)</f>
+        <f t="shared" si="1"/>
         <v>Gittins, Harry</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
@@ -3418,14 +3415,14 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G62:H62)</f>
+        <f t="shared" si="1"/>
         <v>Govenlock, William</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
@@ -3441,14 +3438,14 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G63:H63)</f>
+        <f t="shared" si="1"/>
         <v>Henderson, Owen</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>335</v>
@@ -3464,14 +3461,14 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G64:H64)</f>
+        <f t="shared" si="1"/>
         <v>Horan, Oliver</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C64" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -3487,14 +3484,14 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G65:H65)</f>
+        <f t="shared" si="1"/>
         <v>Humphries, Will</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C65" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -3508,14 +3505,14 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G66:H66)</f>
+        <f t="shared" ref="A66:A97" si="2">_xlfn.TEXTJOIN(", ",1,G66:H66)</f>
         <v>Jamieson, Anna</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>184</v>
@@ -3531,14 +3528,14 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G67:H67)</f>
+        <f t="shared" si="2"/>
         <v>Jassal, Xavier</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C67" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
@@ -3554,14 +3551,14 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G68:H68)</f>
+        <f t="shared" si="2"/>
         <v>Joy, Ben</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C68" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>338</v>
@@ -3577,14 +3574,14 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G69:H69)</f>
+        <f t="shared" si="2"/>
         <v>Lee, Andrew</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C69" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
@@ -3602,14 +3599,14 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G70:H70)</f>
+        <f t="shared" si="2"/>
         <v>Loverso, Liam</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C70" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>182</v>
@@ -3625,14 +3622,14 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G71:H71)</f>
+        <f t="shared" si="2"/>
         <v>May, Heidi</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C71" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>186</v>
@@ -3650,14 +3647,14 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G72:H72)</f>
+        <f t="shared" si="2"/>
         <v>Parker, Cameron</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C72" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
@@ -3673,14 +3670,14 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G73:H73)</f>
+        <f t="shared" si="2"/>
         <v>Sandy, John</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3694,14 +3691,14 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G74:H74)</f>
+        <f t="shared" si="2"/>
         <v>Stacey, Liam</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C74" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
@@ -3717,19 +3714,19 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G75:H75)</f>
+        <f t="shared" si="2"/>
         <v>Tassiopoulos, Emily</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>131</v>
@@ -3740,14 +3737,14 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G76:H76)</f>
+        <f t="shared" si="2"/>
         <v>Taylor, John</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -3761,14 +3758,14 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G77:H77)</f>
+        <f t="shared" si="2"/>
         <v>Zvirbulis, Tom</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C77" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>367</v>
@@ -3784,14 +3781,14 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G78:H78)</f>
+        <f t="shared" si="2"/>
         <v>Fraser, Henry</v>
       </c>
       <c r="B78" s="38" t="s">
         <v>342</v>
       </c>
       <c r="C78" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D78" s="17" t="s">
         <v>343</v>
@@ -3807,14 +3804,14 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G79:H79)</f>
+        <f t="shared" si="2"/>
         <v>Mccarthy, Tess</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C79" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>332</v>
@@ -3830,14 +3827,14 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G80:H80)</f>
+        <f t="shared" si="2"/>
         <v>Alleva, Amelie</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>369</v>
       </c>
       <c r="C80" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>368</v>
@@ -3853,14 +3850,14 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G81:H81)</f>
+        <f t="shared" si="2"/>
         <v>Blackman, Jamie</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>369</v>
       </c>
       <c r="C81" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>359</v>
@@ -3876,14 +3873,14 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G82:H82)</f>
+        <f t="shared" si="2"/>
         <v>Grave, Fergus</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>369</v>
       </c>
       <c r="C82" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="17" t="s">
@@ -3899,14 +3896,14 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G83:H83)</f>
+        <f t="shared" si="2"/>
         <v>Kenny, Angus</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>369</v>
       </c>
       <c r="C83" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>339</v>
@@ -3914,7 +3911,7 @@
       <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>17</v>
@@ -3922,14 +3919,14 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G84:H84)</f>
+        <f t="shared" si="2"/>
         <v>Alleva, James</v>
       </c>
       <c r="B84" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C84" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D84" s="17" t="s">
         <v>345</v>
@@ -3945,14 +3942,14 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G85:H85)</f>
+        <f t="shared" si="2"/>
         <v>Blake, Angus</v>
       </c>
       <c r="B85" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C85" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D85" s="17" t="s">
         <v>341</v>
@@ -3968,14 +3965,14 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G86:H86)</f>
+        <f t="shared" si="2"/>
         <v>Bodon, Maximus</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C86" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -3989,14 +3986,14 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G87:H87)</f>
+        <f t="shared" si="2"/>
         <v>Dytor, Campbell</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C87" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>370</v>
@@ -4012,14 +4009,14 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G88:H88)</f>
+        <f t="shared" si="2"/>
         <v>Edney, Sam</v>
       </c>
       <c r="B88" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C88" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -4033,14 +4030,14 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G89:H89)</f>
+        <f t="shared" si="2"/>
         <v>Edney, William</v>
       </c>
       <c r="B89" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C89" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -4054,14 +4051,14 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G90:H90)</f>
+        <f t="shared" si="2"/>
         <v>Egerton, James</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C90" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D90" s="17" t="s">
         <v>329</v>
@@ -4077,14 +4074,14 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G91:H91)</f>
+        <f t="shared" si="2"/>
         <v>Harmon, Edward</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C91" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
@@ -4100,14 +4097,14 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G92:H92)</f>
+        <f t="shared" si="2"/>
         <v>Hearn, William</v>
       </c>
       <c r="B92" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C92" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>194</v>
@@ -4123,14 +4120,14 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G93:H93)</f>
+        <f t="shared" si="2"/>
         <v>Hoath, Oscar</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C93" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="17" t="s">
@@ -4146,14 +4143,14 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G94:H94)</f>
+        <f t="shared" si="2"/>
         <v>Hogan, Daniel</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C94" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -4167,14 +4164,14 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G95:H95)</f>
+        <f t="shared" si="2"/>
         <v>Johnson, Marcus</v>
       </c>
       <c r="B95" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C95" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>337</v>
@@ -4190,77 +4187,77 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G96:H96)</f>
+        <f t="shared" si="2"/>
         <v>Langford, Cohen</v>
       </c>
       <c r="B96" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C96" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="5"/>
       <c r="G96" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="H96" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G97:H97)</f>
+        <f t="shared" si="2"/>
         <v>Langford, Ellis</v>
       </c>
       <c r="B97" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C97" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="5"/>
       <c r="G97" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="23" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G98:H98)</f>
+        <f t="shared" ref="A98:A121" si="3">_xlfn.TEXTJOIN(", ",1,G98:H98)</f>
         <v>Leeton, Fred</v>
       </c>
       <c r="B98" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C98" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="5"/>
       <c r="G98" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="H98" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G99:H99)</f>
+        <f t="shared" si="3"/>
         <v>Macdonald, Lachie</v>
       </c>
       <c r="B99" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C99" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>345</v>
@@ -4276,14 +4273,14 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G100:H100)</f>
+        <f t="shared" si="3"/>
         <v>Mcdonald, James</v>
       </c>
       <c r="B100" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C100" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -4297,14 +4294,14 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G101:H101)</f>
+        <f t="shared" si="3"/>
         <v>Mclisky, James</v>
       </c>
       <c r="B101" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C101" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D101" s="17" t="s">
         <v>374</v>
@@ -4312,7 +4309,7 @@
       <c r="E101" s="4"/>
       <c r="F101" s="5"/>
       <c r="G101" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>6</v>
@@ -4320,14 +4317,14 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G102:H102)</f>
+        <f t="shared" si="3"/>
         <v>Milo, Freya</v>
       </c>
       <c r="B102" s="38" t="s">
         <v>181</v>
       </c>
       <c r="C102" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D102" s="17" t="s">
         <v>330</v>
@@ -4335,22 +4332,22 @@
       <c r="E102" s="4"/>
       <c r="F102" s="5"/>
       <c r="G102" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="H102" s="5" t="s">
         <v>414</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G103:H103)</f>
+        <f t="shared" si="3"/>
         <v>Parsons, Angus</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C103" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -4364,14 +4361,14 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G104:H104)</f>
+        <f t="shared" si="3"/>
         <v>Perry, Nicholas</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C104" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D104" s="17" t="s">
         <v>331</v>
@@ -4387,14 +4384,14 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G105:H105)</f>
+        <f t="shared" si="3"/>
         <v>Poustie, Sarah</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C105" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D105" s="17" t="s">
         <v>334</v>
@@ -4410,14 +4407,14 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G106:H106)</f>
+        <f t="shared" si="3"/>
         <v>Skinner, Max</v>
       </c>
       <c r="B106" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C106" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D106" s="17" t="s">
         <v>345</v>
@@ -4433,14 +4430,14 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G107:H107)</f>
+        <f t="shared" si="3"/>
         <v>Smith, Jackson</v>
       </c>
       <c r="B107" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C107" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -4454,14 +4451,14 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G108:H108)</f>
+        <f t="shared" si="3"/>
         <v>Spowart, Talei</v>
       </c>
       <c r="B108" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C108" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>184</v>
@@ -4477,14 +4474,14 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G109:H109)</f>
+        <f t="shared" si="3"/>
         <v>Steele, Henry</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C109" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>336</v>
@@ -4500,14 +4497,14 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G110:H110)</f>
+        <f t="shared" si="3"/>
         <v>Sutherland, Finlay</v>
       </c>
       <c r="B110" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D110" s="17" t="s">
         <v>328</v>
@@ -4523,14 +4520,14 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G111:H111)</f>
+        <f t="shared" si="3"/>
         <v>Wood, Bridie</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C111" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D111" s="17" t="s">
         <v>184</v>
@@ -4546,14 +4543,14 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G112:H112)</f>
+        <f t="shared" si="3"/>
         <v>Blaikie, Ben</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C112" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -4567,14 +4564,14 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G113:H113)</f>
+        <f t="shared" si="3"/>
         <v>Mcdonell, Ben</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C113" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -4588,14 +4585,14 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G114:H114)</f>
+        <f t="shared" si="3"/>
         <v>Minisini, Annabella</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C114" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -4609,14 +4606,14 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G115:H115)</f>
+        <f t="shared" si="3"/>
         <v>Mohamed, Abdulkadir</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C115" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -4630,14 +4627,14 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G116:H116)</f>
+        <f t="shared" si="3"/>
         <v>Thorne, James</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C116" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -4651,14 +4648,14 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G117:H117)</f>
+        <f t="shared" si="3"/>
         <v>Gale, Ryan</v>
       </c>
       <c r="B117" s="36" t="s">
         <v>162</v>
       </c>
       <c r="C117" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -4672,14 +4669,14 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G118:H118)</f>
+        <f t="shared" si="3"/>
         <v>Horan, Finn</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C118" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
@@ -4695,14 +4692,14 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G119:H119)</f>
+        <f t="shared" si="3"/>
         <v>Jones, Louis</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C119" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D119" s="17"/>
       <c r="E119" s="4" t="s">
@@ -4710,22 +4707,22 @@
       </c>
       <c r="F119" s="37"/>
       <c r="G119" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="H119" s="5" t="s">
         <v>410</v>
-      </c>
-      <c r="H119" s="5" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G120:H120)</f>
+        <f t="shared" si="3"/>
         <v>Moore, Jennifer</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C120" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -4739,14 +4736,14 @@
     </row>
     <row r="121" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="str">
-        <f>_xlfn.TEXTJOIN(", ",1,G121:H121)</f>
+        <f t="shared" si="3"/>
         <v>Ravi, Rohan</v>
       </c>
       <c r="B121" s="39" t="s">
         <v>162</v>
       </c>
       <c r="C121" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>333</v>
@@ -4761,13 +4758,6 @@
       <c r="H121" s="7" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="4"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H121" xr:uid="{7C87B008-240E-EE4F-AB8D-3B047222A841}">
@@ -4784,10 +4774,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:FG127"/>
+  <dimension ref="A1:FG119"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView topLeftCell="A97" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U122" sqref="U122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4834,7 +4824,7 @@
         <v>172</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>173</v>
@@ -4852,7 +4842,7 @@
         <v>177</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R1" s="14" t="s">
         <v>178</v>
@@ -5285,7 +5275,7 @@
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -5644,7 +5634,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S24" s="5"/>
     </row>
@@ -5671,7 +5661,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S25" s="5"/>
     </row>
@@ -5893,7 +5883,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -6527,7 +6517,7 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -6547,7 +6537,7 @@
       </c>
       <c r="N58" s="4"/>
       <c r="O58" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P58" s="4"/>
       <c r="Q58" s="4"/>
@@ -6556,7 +6546,7 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -6576,7 +6566,7 @@
       </c>
       <c r="N59" s="4"/>
       <c r="O59" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
@@ -6603,7 +6593,7 @@
         <v>379</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -6832,7 +6822,7 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -6946,7 +6936,7 @@
         <v>183</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
@@ -6973,7 +6963,7 @@
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
@@ -7000,7 +6990,7 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
@@ -7086,7 +7076,7 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -7254,7 +7244,7 @@
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
@@ -7355,7 +7345,7 @@
       </c>
       <c r="I89" s="4"/>
       <c r="J89" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K89" s="17"/>
       <c r="L89" s="4"/>
@@ -7561,10 +7551,10 @@
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
       <c r="J97" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K97" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
@@ -8126,86 +8116,6 @@
       <c r="Q119" s="4"/>
       <c r="R119" s="4"/>
       <c r="S119" s="5"/>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
-      <c r="B120" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
-      <c r="J120" s="4"/>
-      <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-      <c r="S120" s="5"/>
-    </row>
-    <row r="121" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="7"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="4"/>
-      <c r="J121" s="4"/>
-      <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-      <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-      <c r="S121" s="5"/>
-    </row>
-    <row r="122" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="8"/>
-      <c r="B122" s="6"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="6"/>
-      <c r="I122" s="6"/>
-      <c r="J122" s="6"/>
-      <c r="K122" s="6"/>
-      <c r="L122" s="6"/>
-      <c r="M122" s="6"/>
-      <c r="N122" s="6"/>
-      <c r="O122" s="6"/>
-      <c r="P122" s="6"/>
-      <c r="Q122" s="6"/>
-      <c r="R122" s="6"/>
-      <c r="S122" s="7"/>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H125" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E126" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E127" t="s">
-        <v>183</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S122" xr:uid="{CF4D3A24-44F2-ED42-B803-827A6EE142F6}">
@@ -8282,7 +8192,7 @@
         <v>181</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -8293,7 +8203,7 @@
         <v>369</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -8320,11 +8230,11 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -8340,7 +8250,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>339</v>
@@ -8374,7 +8284,7 @@
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -8520,7 +8430,7 @@
         <v>181</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -8724,15 +8634,15 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>